<commit_message>
create robot generate result report
</commit_message>
<xml_diff>
--- a/data_magento.xlsx
+++ b/data_magento.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -528,7 +528,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -639,7 +639,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -750,7 +750,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -772,7 +772,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -883,7 +883,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -898,7 +898,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -935,7 +935,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -972,7 +972,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -994,7 +994,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>000002745</t>
+          <t>000003810</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>23:05:19 2024-05-21</t>
+          <t>09:41:06 2024-05-28</t>
         </is>
       </c>
     </row>

</xml_diff>